<commit_message>
all functions of admin is done
</commit_message>
<xml_diff>
--- a/upload/student_list.xlsx
+++ b/upload/student_list.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Capstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\xampp\htdocs\SPM_Final\upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F273A04-9416-4EE5-AF01-261EEC8CF51A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{59D8D38E-6B0A-4728-958D-472EE09D0F5D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7395" xr2:uid="{81562721-A1B2-458C-A7DE-070BAB01082F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Name</t>
   </si>
@@ -51,30 +51,6 @@
     <t>SE02312</t>
   </si>
   <si>
-    <t>SE02313</t>
-  </si>
-  <si>
-    <t>SE02314</t>
-  </si>
-  <si>
-    <t>SE02315</t>
-  </si>
-  <si>
-    <t>SE02316</t>
-  </si>
-  <si>
-    <t>SE02317</t>
-  </si>
-  <si>
-    <t>SE02318</t>
-  </si>
-  <si>
-    <t>SE02319</t>
-  </si>
-  <si>
-    <t>SE02320</t>
-  </si>
-  <si>
     <t>SE02321</t>
   </si>
   <si>
@@ -87,103 +63,25 @@
     <t xml:space="preserve"> ES</t>
   </si>
   <si>
-    <t xml:space="preserve"> IA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0123378290 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> JS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0123782537 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">IS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0123833426 </t>
-  </si>
-  <si>
     <t>Tran Van A</t>
   </si>
   <si>
-    <t>Tran Van B</t>
-  </si>
-  <si>
-    <t>Tran Van C</t>
-  </si>
-  <si>
-    <t>Tran Van D</t>
-  </si>
-  <si>
-    <t>Tran Van E</t>
-  </si>
-  <si>
-    <t>Nguyen Thi A</t>
-  </si>
-  <si>
-    <t>Nguyen Thi B</t>
-  </si>
-  <si>
-    <t>Nguyen Thi C</t>
-  </si>
-  <si>
-    <t>Nguyen Thi D</t>
-  </si>
-  <si>
     <t>Nguyen Thi E</t>
   </si>
   <si>
     <t>avtSE02312@fpt.edu.vn</t>
   </si>
   <si>
-    <t>bvtSE02313@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>cvtSE02314@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>dvtSE02315@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>evtSE02316@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>antSE02317@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>bntSE02318@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>cntSE02319@fpt.edu.vn</t>
-  </si>
-  <si>
-    <t>dntSE02320@fpt.edu.vn</t>
-  </si>
-  <si>
     <t>entSE02321@fpt.edu.vn</t>
   </si>
   <si>
-    <t>0983700283</t>
-  </si>
-  <si>
-    <t>0987139094</t>
-  </si>
-  <si>
     <t>0985359340</t>
   </si>
   <si>
-    <t xml:space="preserve">0919880386 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0910234118 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">0914359440 </t>
-  </si>
-  <si>
     <t xml:space="preserve">0914310156 </t>
+  </si>
+  <si>
+    <t>IS</t>
   </si>
 </sst>
 </file>
@@ -191,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="[&lt;=9999999][$-1000000]###\-####;[$-1000000]\(#\)\ ###\-####"/>
+    <numFmt numFmtId="164" formatCode="[&lt;=9999999][$-1000000]###\-####;[$-1000000]\(#\)\ ###\-####"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -251,8 +149,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -597,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C0550F-2013-4381-8714-14CBFE6F8E2A}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" activeCellId="1" sqref="F14 H9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,22 +539,22 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2">
         <v>33211</v>
       </c>
       <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>52</v>
-      </c>
       <c r="F2" s="4" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -664,225 +562,82 @@
         <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2">
-        <v>33872</v>
+        <v>35250</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="2">
-        <v>33943</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="2"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2">
-        <v>34411</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="2">
-        <v>34424</v>
-      </c>
-      <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="2"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="2">
-        <v>34736</v>
-      </c>
-      <c r="D7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="2"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" s="2">
-        <v>34784</v>
-      </c>
-      <c r="D8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="2"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="3"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2">
-        <v>35088</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="2"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="2">
-        <v>35149</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" s="2">
-        <v>35250</v>
-      </c>
-      <c r="D11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="2"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{423DE728-0DF9-475F-8308-C20BC10FE084}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{2B5AC18A-FB6F-4E4A-9A53-4585BC22A043}"/>
-    <hyperlink ref="F4" r:id="rId3" xr:uid="{E44A619E-8362-48F2-9C10-980C35596EC7}"/>
-    <hyperlink ref="F5" r:id="rId4" xr:uid="{7EB07B43-1753-46B7-A134-A5E79BAB1962}"/>
-    <hyperlink ref="F6" r:id="rId5" xr:uid="{0BAD04A4-3579-4013-BCEF-7A16C7792876}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{E0FBB3AC-3FEE-4173-8A00-48B4E3260931}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{1239D04B-5E72-4162-BE98-DB09A7119514}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{F29D3DA8-B236-4DDD-84EF-B7EE37394F90}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{E90AE367-7043-4CA8-AA34-3D5BA637B28E}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{9A43DC40-755A-4995-8AC5-0E0BF16C1EBF}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{9A43DC40-755A-4995-8AC5-0E0BF16C1EBF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId11"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <ignoredErrors>
-    <ignoredError sqref="E10 E11 E7 E8 E3 E4 E2 E5:E6 E9" numberStoredAsText="1"/>
+    <ignoredError sqref="E2" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>